<commit_message>
Language update and debug
</commit_message>
<xml_diff>
--- a/20240801_線上問卷中英葡文內容_DSAT.xlsx
+++ b/20240801_線上問卷中英葡文內容_DSAT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianNg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Downloads\GitHub\tswebsurvey_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D068E25-C8C8-4622-A2A8-EEE5F4CF407C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="9075" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="1" r:id="rId1"/>
@@ -30,28 +31,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Brian, Ng Kuok Hou</author>
   </authors>
   <commentList>
-    <comment ref="A22" authorId="0" shapeId="0">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="588">
   <si>
     <t>中文</t>
   </si>
@@ -2201,12 +2191,28 @@
     </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>請填寫其他的通關口岸</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>請填寫其他</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>請選擇回家使用的通關口岸</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>請填寫其他通關口岸</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2320,6 +2326,13 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2359,25 +2372,23 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -2711,7 +2722,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -2811,7 +2822,7 @@
       <c r="B8" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>572</v>
       </c>
     </row>
@@ -2822,7 +2833,7 @@
       <c r="B9" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>568</v>
       </c>
     </row>
@@ -2877,7 +2888,7 @@
       <c r="B14" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>573</v>
       </c>
     </row>
@@ -2889,7 +2900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="工作表10"/>
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3076,7 +3087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="工作表11"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -3187,7 +3198,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="工作表12"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3229,7 +3240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="工作表2"/>
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -3484,7 +3495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="工作表3"/>
   <dimension ref="A1:C39"/>
   <sheetViews>
@@ -3936,7 +3947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="工作表4"/>
   <dimension ref="A1:C34"/>
   <sheetViews>
@@ -4325,7 +4336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="工作表5"/>
   <dimension ref="A1:C61"/>
   <sheetViews>
@@ -4375,7 +4386,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -4386,7 +4397,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -5019,12 +5030,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="工作表6"/>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5574,6 +5585,16 @@
         <v>576</v>
       </c>
     </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="13" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5582,12 +5603,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="工作表7"/>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5621,7 +5642,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="3" t="s">
         <v>155</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -6322,6 +6343,16 @@
       </c>
       <c r="C66" s="7" t="s">
         <v>516</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="3" t="s">
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -6331,11 +6362,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="工作表8"/>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -6620,7 +6651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="工作表9"/>
   <dimension ref="A1:C13"/>
   <sheetViews>

</xml_diff>